<commit_message>
fixed severe PCB issue, clearance of ground fills was too small, could lead to thermal instability
</commit_message>
<xml_diff>
--- a/hw/pcb/bom.xlsx
+++ b/hw/pcb/bom.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="164">
   <si>
     <t>Designator</t>
   </si>
@@ -103,9 +103,6 @@
     <t>2k2</t>
   </si>
   <si>
-    <t>R301</t>
-  </si>
-  <si>
     <t>470R</t>
   </si>
   <si>
@@ -256,9 +253,6 @@
     <t>THONKICONN</t>
   </si>
   <si>
-    <t>J501</t>
-  </si>
-  <si>
     <t>PinHeader_2x05_P2.54mm_Vertical_SMD</t>
   </si>
   <si>
@@ -497,6 +491,21 @@
   </si>
   <si>
     <t>Q302,Q301,Q602,Q601</t>
+  </si>
+  <si>
+    <t>4k7</t>
+  </si>
+  <si>
+    <t>R304</t>
+  </si>
+  <si>
+    <t>C25900</t>
+  </si>
+  <si>
+    <t>R301, R305</t>
+  </si>
+  <si>
+    <t>J101</t>
   </si>
 </sst>
 </file>
@@ -1354,10 +1363,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G47"/>
+  <dimension ref="A1:G48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="E52" sqref="E52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1370,25 +1379,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
@@ -1396,7 +1405,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>9</v>
@@ -1405,13 +1414,13 @@
         <v>1</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="G2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
@@ -1420,46 +1429,46 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="G3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
-        <f t="shared" ref="A4:A32" si="0">A3+1</f>
+        <f t="shared" ref="A4:A33" si="0">A3+1</f>
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D4">
         <v>19</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
@@ -1468,22 +1477,22 @@
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D5">
         <v>5</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="G5" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
@@ -1492,7 +1501,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>1</v>
@@ -1504,10 +1513,10 @@
         <v>2</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G6" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
@@ -1516,7 +1525,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>4</v>
@@ -1528,10 +1537,10 @@
         <v>5</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
@@ -1552,10 +1561,10 @@
         <v>7</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G8" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
@@ -1564,7 +1573,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>10</v>
@@ -1576,10 +1585,10 @@
         <v>11</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="G9" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
@@ -1588,10 +1597,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D10">
         <v>2</v>
@@ -1600,10 +1609,10 @@
         <v>12</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G10" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
@@ -1612,10 +1621,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D11">
         <v>2</v>
@@ -1624,10 +1633,10 @@
         <v>12</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G11" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
@@ -1648,10 +1657,10 @@
         <v>12</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
@@ -1660,7 +1669,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>16</v>
@@ -1672,10 +1681,10 @@
         <v>12</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G13" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
@@ -1687,7 +1696,7 @@
         <v>13</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D14">
         <v>5</v>
@@ -1696,10 +1705,10 @@
         <v>12</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="G14" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
@@ -1720,10 +1729,10 @@
         <v>12</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G15" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
@@ -1744,70 +1753,67 @@
         <v>12</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G16" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A17" s="3">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
+        <v>92</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" s="4" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A17" s="3"/>
       <c r="B17" s="4" t="s">
-        <v>22</v>
+        <v>159</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D17">
-        <v>6</v>
+        <v>160</v>
+      </c>
+      <c r="D17" s="4">
+        <v>1</v>
       </c>
       <c r="E17" s="4" t="s">
         <v>12</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="G17" t="s">
-        <v>94</v>
+        <v>161</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
-        <f t="shared" si="0"/>
-        <v>17</v>
+        <f>A16+1</f>
+        <v>16</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D18">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>12</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="G18" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D19">
         <v>2</v>
@@ -1816,46 +1822,46 @@
         <v>12</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="G19" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D20">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E20" s="4" t="s">
         <v>12</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="G20" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D21">
         <v>1</v>
@@ -1864,641 +1870,665 @@
         <v>12</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="G21" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
         <f t="shared" si="0"/>
-        <v>21</v>
-      </c>
-      <c r="B22" s="4">
-        <v>680</v>
+        <v>20</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>29</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>31</v>
+        <v>162</v>
       </c>
       <c r="D22">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E22" s="4" t="s">
         <v>12</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="G22" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
         <f t="shared" si="0"/>
-        <v>22</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>32</v>
+        <v>21</v>
+      </c>
+      <c r="B23" s="4">
+        <v>680</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>160</v>
+        <v>30</v>
       </c>
       <c r="D23">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="G23" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
-        <f>A23+1</f>
-        <v>23</v>
-      </c>
-      <c r="B24" s="4">
-        <v>600</v>
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>31</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>33</v>
+        <v>158</v>
       </c>
       <c r="D24">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>34</v>
+        <v>3</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="G24" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
-        <f t="shared" si="0"/>
-        <v>24</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>37</v>
+        <f>A24+1</f>
+        <v>23</v>
+      </c>
+      <c r="B25" s="4">
+        <v>600</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="G25" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
         <f t="shared" si="0"/>
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>87</v>
+        <v>36</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D26">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="G26" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
         <f t="shared" si="0"/>
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>41</v>
+        <v>85</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>158</v>
+        <v>39</v>
       </c>
       <c r="D27">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="G27" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A28" s="3">
         <f t="shared" si="0"/>
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D28">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="G28" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A29" s="3">
         <f t="shared" si="0"/>
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>43</v>
+        <v>157</v>
       </c>
       <c r="D29">
         <v>2</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="G29" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A30" s="3">
         <f t="shared" si="0"/>
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D30">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="G30" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A31" s="3">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D31">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>120</v>
+        <v>117</v>
+      </c>
+      <c r="G31" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A32" s="3">
         <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D32">
+        <v>3</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A33" s="3">
+        <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="B32" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="C32" s="4" t="s">
+      <c r="B33" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D32">
+      <c r="C33" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D33">
         <v>1</v>
       </c>
-      <c r="E32" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="F32" s="5" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="3">
-        <f>A32+1</f>
-        <v>32</v>
-      </c>
-      <c r="B33" t="s">
-        <v>53</v>
-      </c>
-      <c r="C33" t="s">
-        <v>51</v>
-      </c>
-      <c r="D33">
-        <f t="shared" ref="D33:D47" si="1">LEN(C33)-LEN(SUBSTITUTE(C33,",",""))+1</f>
-        <v>1</v>
-      </c>
-      <c r="E33" t="s">
-        <v>52</v>
-      </c>
-      <c r="F33" t="s">
-        <v>142</v>
-      </c>
-      <c r="G33" t="s">
-        <v>131</v>
+      <c r="E33" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
-        <f t="shared" ref="A34:A47" si="2">A33+1</f>
-        <v>33</v>
+        <f>A33+1</f>
+        <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C34" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D34">
-        <f t="shared" si="1"/>
-        <v>2</v>
+        <f t="shared" ref="D34:D48" si="1">LEN(C34)-LEN(SUBSTITUTE(C34,",",""))+1</f>
+        <v>1</v>
       </c>
       <c r="E34" t="s">
-        <v>55</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>136</v>
+        <v>51</v>
+      </c>
+      <c r="F34" t="s">
+        <v>140</v>
       </c>
       <c r="G34" t="s">
-        <v>143</v>
+        <v>129</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
-        <f t="shared" si="2"/>
-        <v>34</v>
+        <f t="shared" ref="A35:A48" si="2">A34+1</f>
+        <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>13</v>
+        <v>55</v>
       </c>
       <c r="C35" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D35">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="E35" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="G35" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <f t="shared" si="2"/>
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>60</v>
+        <v>13</v>
       </c>
       <c r="C36" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D36">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E36" t="s">
-        <v>59</v>
-      </c>
-      <c r="F36" t="s">
-        <v>138</v>
+        <v>54</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>135</v>
       </c>
       <c r="G36" t="s">
-        <v>131</v>
+        <v>141</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <f t="shared" si="2"/>
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C37" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D37">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="E37" t="s">
-        <v>3</v>
+        <v>58</v>
       </c>
       <c r="F37" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="G37" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
         <f t="shared" si="2"/>
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C38" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D38">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="E38" t="s">
-        <v>64</v>
+        <v>3</v>
       </c>
       <c r="F38" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="G38" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <f t="shared" si="2"/>
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C39" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D39">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="E39" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F39" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="G39" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
-        <f>A38+1</f>
+        <f t="shared" si="2"/>
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C40" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D40">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E40" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F40" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="G40" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <f>A39+1</f>
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B41" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C41" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D41">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="E41" t="s">
-        <v>69</v>
-      </c>
-      <c r="F41" s="2" t="s">
-        <v>135</v>
+        <v>68</v>
+      </c>
+      <c r="F41" t="s">
+        <v>132</v>
       </c>
       <c r="G41" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
-        <f t="shared" si="2"/>
-        <v>40</v>
+        <f>A40+1</f>
+        <v>39</v>
       </c>
       <c r="B42" t="s">
-        <v>124</v>
+        <v>69</v>
       </c>
       <c r="C42" t="s">
-        <v>123</v>
+        <v>67</v>
       </c>
       <c r="D42">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E42" t="s">
-        <v>79</v>
-      </c>
-      <c r="F42" s="1" t="s">
-        <v>128</v>
+        <v>68</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="G42" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <f t="shared" si="2"/>
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B43" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C43" t="s">
-        <v>80</v>
+        <v>121</v>
       </c>
       <c r="D43">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="E43" t="s">
-        <v>81</v>
-      </c>
-      <c r="F43" t="s">
-        <v>129</v>
+        <v>78</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
         <f t="shared" si="2"/>
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B44" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C44" t="s">
-        <v>82</v>
+        <v>163</v>
       </c>
       <c r="D44">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="E44" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="F44" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
         <f t="shared" si="2"/>
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B45" t="s">
-        <v>86</v>
+        <v>123</v>
       </c>
       <c r="C45" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D45">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="E45" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="F45" t="s">
-        <v>130</v>
-      </c>
-      <c r="G45" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
         <f t="shared" si="2"/>
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B46" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="C46" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="D46">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="E46" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="F46" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="G46" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
         <f t="shared" si="2"/>
-        <v>45</v>
-      </c>
-      <c r="B47">
-        <v>10</v>
+        <v>44</v>
+      </c>
+      <c r="B47" t="s">
+        <v>88</v>
       </c>
       <c r="C47" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="D47">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="E47" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="F47" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="G47" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="3">
+        <f t="shared" si="2"/>
+        <v>45</v>
+      </c>
+      <c r="B48">
+        <v>10</v>
+      </c>
+      <c r="C48" t="s">
+        <v>76</v>
+      </c>
+      <c r="D48">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E48" t="s">
+        <v>77</v>
+      </c>
+      <c r="F48" t="s">
         <v>131</v>
+      </c>
+      <c r="G48" t="s">
+        <v>129</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F42" r:id="rId1"/>
-    <hyperlink ref="F34" r:id="rId2"/>
-    <hyperlink ref="F35" r:id="rId3"/>
+    <hyperlink ref="F43" r:id="rId1"/>
+    <hyperlink ref="F35" r:id="rId2"/>
+    <hyperlink ref="F36" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId4"/>

</xml_diff>